<commit_message>
Completed Collected Specimen in Diagnostic Report IG
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/specimen-collect-1.xlsx
+++ b/output/DiagnosticReport/specimen-collect-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2336" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2336" uniqueCount="361">
   <si>
     <t>Path</t>
   </si>
@@ -150,7 +150,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}inv-dh-spc-01:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt; 1).exists()}</t>
   </si>
   <si>
     <t>Role[classCode=SPEC]</t>
@@ -546,7 +546,7 @@
     <t>Specimen.subject</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/patient-ident-1|http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/patient-mhr-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/patient-ident-1|http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/patient-mhr-1)
 </t>
   </si>
   <si>
@@ -644,6 +644,10 @@
     <t>Details concerning the specimen collection.</t>
   </si>
   <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+inv-dh-spc-02:If present, the collector shall at least have a reference or an identifier with at least a system and a value {collector.exists() implies collector.reference.exists() or collector.identifier.where(system.count() + value.count() &gt;1).exists()}</t>
+  </si>
+  <si>
     <t>.participation[typeCode=SBJ].act[classCode=SPECCOLLECT, moodCode=EVN]</t>
   </si>
   <si>
@@ -676,7 +680,7 @@
     <t>Specimen.collection.collector</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/practitionerrole-ident-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/practitionerrole-ident-1)
 </t>
   </si>
   <si>
@@ -3906,21 +3910,21 @@
         <v>39</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>59</v>
+        <v>201</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="AK24" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4026,7 +4030,7 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4134,11 +4138,11 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
@@ -4160,10 +4164,10 @@
         <v>93</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="M27" t="s" s="2">
         <v>96</v>
@@ -4218,7 +4222,7 @@
         <v>39</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>40</v>
@@ -4244,7 +4248,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4267,13 +4271,13 @@
         <v>48</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -4324,7 +4328,7 @@
         <v>39</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>40</v>
@@ -4339,18 +4343,18 @@
         <v>59</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4373,13 +4377,13 @@
         <v>48</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -4430,7 +4434,7 @@
         <v>39</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>40</v>
@@ -4445,18 +4449,18 @@
         <v>59</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4479,13 +4483,13 @@
         <v>48</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -4536,7 +4540,7 @@
         <v>39</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>40</v>
@@ -4554,7 +4558,7 @@
         <v>39</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>39</v>
@@ -4562,7 +4566,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4585,13 +4589,13 @@
         <v>39</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -4642,7 +4646,7 @@
         <v>39</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>40</v>
@@ -4657,18 +4661,18 @@
         <v>59</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AK31" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4694,10 +4698,10 @@
         <v>127</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -4727,10 +4731,10 @@
         <v>131</v>
       </c>
       <c r="X32" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="Y32" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="Z32" t="s" s="2">
         <v>39</v>
@@ -4748,7 +4752,7 @@
         <v>39</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>40</v>
@@ -4763,18 +4767,18 @@
         <v>59</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AK32" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -4880,7 +4884,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -4988,7 +4992,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5096,10 +5100,10 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C36" t="s" s="2">
         <v>39</v>
@@ -5124,7 +5128,7 @@
         <v>149</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="L36" t="s" s="2">
         <v>151</v>
@@ -5161,10 +5165,10 @@
         <v>120</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Y36" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="Z36" t="s" s="2">
         <v>39</v>
@@ -5208,7 +5212,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5318,7 +5322,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5344,13 +5348,13 @@
         <v>127</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
@@ -5379,10 +5383,10 @@
         <v>131</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>39</v>
@@ -5400,7 +5404,7 @@
         <v>39</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>40</v>
@@ -5415,18 +5419,18 @@
         <v>59</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AK38" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5532,7 +5536,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5640,7 +5644,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5748,10 +5752,10 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C42" t="s" s="2">
         <v>39</v>
@@ -5776,7 +5780,7 @@
         <v>149</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="L42" t="s" s="2">
         <v>151</v>
@@ -5813,10 +5817,10 @@
         <v>120</v>
       </c>
       <c r="X42" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="Y42" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="Z42" t="s" s="2">
         <v>39</v>
@@ -5860,7 +5864,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -5970,7 +5974,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -5993,19 +5997,19 @@
         <v>48</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="N44" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="O44" t="s" s="2">
         <v>39</v>
@@ -6030,13 +6034,13 @@
         <v>39</v>
       </c>
       <c r="W44" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="Z44" t="s" s="2">
         <v>39</v>
@@ -6054,7 +6058,7 @@
         <v>39</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>40</v>
@@ -6075,12 +6079,12 @@
         <v>39</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6106,10 +6110,10 @@
         <v>198</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -6160,7 +6164,7 @@
         <v>39</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>40</v>
@@ -6175,7 +6179,7 @@
         <v>59</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AK45" t="s" s="2">
         <v>39</v>
@@ -6186,7 +6190,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6292,7 +6296,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6400,11 +6404,11 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
@@ -6426,10 +6430,10 @@
         <v>93</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="M48" t="s" s="2">
         <v>96</v>
@@ -6484,7 +6488,7 @@
         <v>39</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>40</v>
@@ -6510,7 +6514,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6536,10 +6540,10 @@
         <v>49</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -6590,7 +6594,7 @@
         <v>39</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>40</v>
@@ -6605,7 +6609,7 @@
         <v>59</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>39</v>
@@ -6616,7 +6620,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6642,10 +6646,10 @@
         <v>127</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -6675,10 +6679,10 @@
         <v>131</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>39</v>
@@ -6696,7 +6700,7 @@
         <v>39</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>40</v>
@@ -6722,7 +6726,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -6745,13 +6749,13 @@
         <v>39</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -6802,7 +6806,7 @@
         <v>39</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>40</v>
@@ -6817,18 +6821,18 @@
         <v>59</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AK51" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -6851,13 +6855,13 @@
         <v>39</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
@@ -6908,7 +6912,7 @@
         <v>39</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>40</v>
@@ -6923,7 +6927,7 @@
         <v>59</v>
       </c>
       <c r="AJ52" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AK52" t="s" s="2">
         <v>39</v>
@@ -6934,7 +6938,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -6960,10 +6964,10 @@
         <v>198</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -7014,7 +7018,7 @@
         <v>39</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>40</v>
@@ -7029,7 +7033,7 @@
         <v>59</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="AK53" t="s" s="2">
         <v>39</v>
@@ -7040,7 +7044,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7146,7 +7150,7 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -7254,11 +7258,11 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" t="s" s="2">
@@ -7280,10 +7284,10 @@
         <v>93</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="M56" t="s" s="2">
         <v>96</v>
@@ -7338,7 +7342,7 @@
         <v>39</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>40</v>
@@ -7364,7 +7368,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7390,10 +7394,10 @@
         <v>105</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -7444,7 +7448,7 @@
         <v>39</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>40</v>
@@ -7465,12 +7469,12 @@
         <v>39</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7496,10 +7500,10 @@
         <v>49</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -7550,7 +7554,7 @@
         <v>39</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>40</v>
@@ -7565,7 +7569,7 @@
         <v>59</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="AK58" t="s" s="2">
         <v>39</v>
@@ -7576,7 +7580,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -7602,10 +7606,10 @@
         <v>127</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -7635,10 +7639,10 @@
         <v>131</v>
       </c>
       <c r="X59" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="Y59" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="Z59" t="s" s="2">
         <v>39</v>
@@ -7656,7 +7660,7 @@
         <v>39</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>40</v>
@@ -7677,12 +7681,12 @@
         <v>39</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -7788,7 +7792,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -7896,7 +7900,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8004,10 +8008,10 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C63" t="s" s="2">
         <v>39</v>
@@ -8032,7 +8036,7 @@
         <v>149</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="L63" t="s" s="2">
         <v>151</v>
@@ -8069,10 +8073,10 @@
         <v>120</v>
       </c>
       <c r="X63" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="Y63" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="Z63" t="s" s="2">
         <v>39</v>
@@ -8116,7 +8120,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8226,7 +8230,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -8249,13 +8253,13 @@
         <v>39</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -8306,7 +8310,7 @@
         <v>39</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>40</v>
@@ -8321,18 +8325,18 @@
         <v>59</v>
       </c>
       <c r="AJ65" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="AK65" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -8355,13 +8359,13 @@
         <v>39</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
@@ -8412,7 +8416,7 @@
         <v>39</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>40</v>
@@ -8427,18 +8431,18 @@
         <v>59</v>
       </c>
       <c r="AJ66" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="AK66" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -8461,13 +8465,13 @@
         <v>39</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -8497,10 +8501,10 @@
         <v>131</v>
       </c>
       <c r="X67" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="Y67" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="Z67" t="s" s="2">
         <v>39</v>
@@ -8518,7 +8522,7 @@
         <v>39</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>40</v>
@@ -8533,18 +8537,18 @@
         <v>59</v>
       </c>
       <c r="AJ67" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AK67" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -8570,16 +8574,16 @@
         <v>127</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="N68" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="O68" t="s" s="2">
         <v>39</v>
@@ -8604,13 +8608,13 @@
         <v>39</v>
       </c>
       <c r="W68" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="X68" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="Y68" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="Z68" t="s" s="2">
         <v>39</v>
@@ -8628,7 +8632,7 @@
         <v>39</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>40</v>
@@ -8649,12 +8653,12 @@
         <v>39</v>
       </c>
       <c r="AL68" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -8677,13 +8681,13 @@
         <v>39</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="K69" t="s" s="2">
         <v>12</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
@@ -8734,7 +8738,7 @@
         <v>39</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>40</v>
@@ -8749,13 +8753,13 @@
         <v>59</v>
       </c>
       <c r="AJ69" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="AK69" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL69" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated output following final fixes for 30th June Project
Final minor fixes to reduce the qa.html errors in the Daignostic Report FHIR IG.
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/specimen-collect-1.xlsx
+++ b/output/DiagnosticReport/specimen-collect-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1648" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1648" uniqueCount="311">
   <si>
     <t>Path</t>
   </si>
@@ -703,6 +703,10 @@
   </si>
   <si>
     <t>https://healthterminologies.gov.au/fhir/ValueSet/body-site-1</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+inv-dh-spc-03:If a coded body site is provided, at least one code shall be from SNOMED CT {coding.exists() implies coding.where(system='http://snomed.info/sct').exists()}</t>
   </si>
   <si>
     <t>.targetSiteCode</t>
@@ -4172,21 +4176,21 @@
         <v>39</v>
       </c>
       <c r="AI28" t="s" s="2">
-        <v>59</v>
+        <v>220</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4209,19 +4213,19 @@
         <v>48</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="O29" t="s" s="2">
         <v>39</v>
@@ -4246,13 +4250,13 @@
         <v>39</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="Y29" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="Z29" t="s" s="2">
         <v>39</v>
@@ -4270,7 +4274,7 @@
         <v>39</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>40</v>
@@ -4291,12 +4295,12 @@
         <v>39</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4322,10 +4326,10 @@
         <v>164</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -4376,7 +4380,7 @@
         <v>39</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>40</v>
@@ -4391,7 +4395,7 @@
         <v>59</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AK30" t="s" s="2">
         <v>39</v>
@@ -4402,7 +4406,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4508,7 +4512,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4616,7 +4620,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -4726,7 +4730,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -4752,10 +4756,10 @@
         <v>49</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -4806,7 +4810,7 @@
         <v>39</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>40</v>
@@ -4821,7 +4825,7 @@
         <v>59</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>39</v>
@@ -4832,7 +4836,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -4858,10 +4862,10 @@
         <v>127</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -4888,13 +4892,13 @@
         <v>39</v>
       </c>
       <c r="W35" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="Z35" t="s" s="2">
         <v>39</v>
@@ -4912,7 +4916,7 @@
         <v>39</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>40</v>
@@ -4938,7 +4942,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -4961,13 +4965,13 @@
         <v>39</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5018,7 +5022,7 @@
         <v>39</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>40</v>
@@ -5033,18 +5037,18 @@
         <v>59</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5070,10 +5074,10 @@
         <v>191</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -5124,7 +5128,7 @@
         <v>39</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>40</v>
@@ -5150,7 +5154,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5176,10 +5180,10 @@
         <v>164</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5230,7 +5234,7 @@
         <v>39</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>40</v>
@@ -5245,7 +5249,7 @@
         <v>59</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AK38" t="s" s="2">
         <v>39</v>
@@ -5256,7 +5260,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5362,7 +5366,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5470,7 +5474,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5580,7 +5584,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -5606,10 +5610,10 @@
         <v>105</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -5660,7 +5664,7 @@
         <v>39</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>40</v>
@@ -5681,12 +5685,12 @@
         <v>39</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -5712,10 +5716,10 @@
         <v>49</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -5766,7 +5770,7 @@
         <v>39</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>40</v>
@@ -5781,7 +5785,7 @@
         <v>59</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="AK43" t="s" s="2">
         <v>39</v>
@@ -5792,7 +5796,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -5818,10 +5822,10 @@
         <v>127</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -5848,13 +5852,13 @@
         <v>39</v>
       </c>
       <c r="W44" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="Z44" t="s" s="2">
         <v>39</v>
@@ -5872,7 +5876,7 @@
         <v>39</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>40</v>
@@ -5893,12 +5897,12 @@
         <v>39</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -5924,10 +5928,10 @@
         <v>202</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -5978,7 +5982,7 @@
         <v>39</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>40</v>
@@ -5993,18 +5997,18 @@
         <v>59</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="AK45" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6030,10 +6034,10 @@
         <v>202</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -6084,7 +6088,7 @@
         <v>39</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>40</v>
@@ -6099,18 +6103,18 @@
         <v>59</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AK46" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6133,13 +6137,13 @@
         <v>39</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -6166,13 +6170,13 @@
         <v>39</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="Z47" t="s" s="2">
         <v>39</v>
@@ -6190,7 +6194,7 @@
         <v>39</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>40</v>
@@ -6205,18 +6209,18 @@
         <v>59</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AK47" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6242,16 +6246,16 @@
         <v>127</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>39</v>
@@ -6276,13 +6280,13 @@
         <v>39</v>
       </c>
       <c r="W48" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="Z48" t="s" s="2">
         <v>39</v>
@@ -6300,7 +6304,7 @@
         <v>39</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>40</v>
@@ -6321,12 +6325,12 @@
         <v>39</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6349,13 +6353,13 @@
         <v>39</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="K49" t="s" s="2">
         <v>12</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -6406,7 +6410,7 @@
         <v>39</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>40</v>
@@ -6421,13 +6425,13 @@
         <v>59</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>